<commit_message>
Add updated example file
</commit_message>
<xml_diff>
--- a/schemas/sequencing_examples_2clauses.xlsx
+++ b/schemas/sequencing_examples_2clauses.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seb/CTDS/Projects/LCT_GPT/code/LCT_sequencing/schemas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seb/CTDS/Projects/LCT_GPT/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E7186EE-B9A9-2348-B533-84278A77963C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE1AA04A-95C0-914C-B06B-63D5A95D5C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="780" windowWidth="33760" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11700" yWindow="1320" windowWidth="25680" windowHeight="14380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,62 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={1470665B-3C43-41A1-9498-59EEAB91EE88}</author>
+    <author>tc={7913A9A6-8C82-4B82-AC9C-24D09A33D601}</author>
+    <author>tc={EF522E50-4973-42D2-8A25-BF3CD1DC3959}</author>
+    <author>tc={5BD9D394-8FAF-477F-B0FD-7B00E365AEEC}</author>
+    <author>tc={CA7BA8EC-4175-4884-91FD-DC948338054D}</author>
+  </authors>
+  <commentList>
+    <comment ref="E10" authorId="0" shapeId="0" xr:uid="{1470665B-3C43-41A1-9498-59EEAB91EE88}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    In each of these chunks, there is in fact another consequential happening - the 'however' links the two chunks here in columns E and F, while the two 'by's link columns G&amp;H and I&amp;J.</t>
+      </text>
+    </comment>
+    <comment ref="E24" authorId="1" shapeId="0" xr:uid="{7913A9A6-8C82-4B82-AC9C-24D09A33D601}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This example has two sets of links, linking three clauses - marked by 'whilst', linking column G&amp;H and 'until', linking columns G&amp;H with I.</t>
+      </text>
+    </comment>
+    <comment ref="E26" authorId="2" shapeId="0" xr:uid="{EF522E50-4973-42D2-8A25-BF3CD1DC3959}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This is an example of an interrupting clause. There is a consequential link between 'When you get trade in ideas' and 'we call it aesthetic trade', but the clause 'you wouldn't have heard this word before' interrupts this link, in a way that we call incoherent sequencing.</t>
+      </text>
+    </comment>
+    <comment ref="D27" authorId="3" shapeId="0" xr:uid="{5BD9D394-8FAF-477F-B0FD-7B00E365AEEC}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    The  |INC… INC| is an annotation of the text, not part of the text itself. Should be removed from the transcript.</t>
+      </text>
+    </comment>
+    <comment ref="E27" authorId="4" shapeId="0" xr:uid="{CA7BA8EC-4175-4884-91FD-DC948338054D}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    As above, this involves an interrupting clause. The is a reiterative relation between 'It doesn't look like this arrangement here' and 'It doesn't look like a full spectrum here', but the clause 'So we'll just turn the lights on again' interrupts this, in a way we label incoherent sequencing.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="196">
   <si>
     <t>Type</t>
   </si>
@@ -61,15 +115,6 @@
     <t>Integrative Sequencing</t>
   </si>
   <si>
-    <t>These findings raise the possibility that regulation of macrophage genes by hdl might link innate immunity and cardioprotection.</t>
-  </si>
-  <si>
-    <t>The use of the linkage word 'These' refers back to previously mentioned findings or results. The statement that follows ('raise the possibility that regulation of macrophage genes by hdl might link innate immunity and cardioprotection') provides an implication or potential significance of the previously mentioned findings. This structure indicates how the initial findings or results are condensed and transported into a new context or perspective, suggesting a potential link between innate immunity and cardioprotection. The relationship between the two passages is established vertically, with the second passage offering a broader implication or significance based on the findings mentioned earlier, thereby condensing and transporting the meanings from the initial context to a new one.</t>
-  </si>
-  <si>
-    <t>these</t>
-  </si>
-  <si>
     <t>No more than one electron in the same atom can have all 4 quantum numbers the same. This is truly wonderful stuff.</t>
   </si>
   <si>
@@ -115,12 +160,6 @@
     <t>then</t>
   </si>
   <si>
-    <t>if we started to look at all the things in Pompeii and Herculaneum, what objects may be showing Greek design? Or Egyptian design? Or Greek mythology? Or Egyptian mythology? Or what building techniques like columns?</t>
-  </si>
-  <si>
-    <t>The use of the linkage word 'if' sets up a conditional scenario, suggesting a hypothetical situation where we examine objects in Pompeii and Herculaneum. The subsequent questions introduced by the word 'Or' present multiple possibilities or alternatives related to the initial scenario. This structure indicates how meanings from different passages shape one another, as each question builds upon the previous one, exploring different facets of the initial hypothetical situation. The use of 'Or' repeatedly emphasizes the various possibilities and alternatives, linking them together in a horizontal sequence.</t>
-  </si>
-  <si>
     <t>If</t>
   </si>
   <si>
@@ -277,15 +316,9 @@
     <t>When you get trade in ideas—you wouldn’t have heard this word before—we call it aesthetic trade</t>
   </si>
   <si>
-    <t>This example juxtaposes two passages that are epistemologically unrelated. The first part discusses the concept of 'trade in ideas', while the interjection 'you wouldn’t have heard this word before' breaks the flow and introduces a commentary on the listener's potential unfamiliarity with the term.</t>
-  </si>
-  <si>
     <t>When</t>
   </si>
   <si>
-    <t>It doesn’t look like this arrangement here. |INC So we’ll just turn the lights on again INC|. It doesn’t look like a full spectrum up here</t>
-  </si>
-  <si>
     <t>incoherent because the middle clause 'So we’ll just turn the lights on again' interrupts the flow of the topic being discussed.  the middle statement about turning the lights on seems unrelated to the surrounding context and introduces a different topic without a clear connection to the preceding or following statement. The use of the continuative 'So' further emphasizes this sudden shift in topic</t>
   </si>
   <si>
@@ -353,13 +386,289 @@
   </si>
   <si>
     <t>Clause_2</t>
+  </si>
+  <si>
+    <t>Linked_Chunk_1</t>
+  </si>
+  <si>
+    <t>Linked_Chunk_2</t>
+  </si>
+  <si>
+    <t>Clause_3</t>
+  </si>
+  <si>
+    <t>Vesicles in the cytoplasm called lysosome fuse with the phagosome releasing digestive enzymes such as lysozyme and proteases into the phagosome.</t>
+  </si>
+  <si>
+    <t>The result of this fusion is called phagolysosome.</t>
+  </si>
+  <si>
+    <t>Vesicles in the cytoplasm called lysosome fuse with the phagosome</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> releasing digestive enzymes such as lysozyme and proteases into the phagosome.</t>
+  </si>
+  <si>
+    <t>No more than one electron in the same atom can have all 4 quantum numbers the same.</t>
+  </si>
+  <si>
+    <t>This is truly wonderful stuff.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The basketball was really flat. </t>
+  </si>
+  <si>
+    <t>That means we can’t play today.</t>
+  </si>
+  <si>
+    <t>Curtsey while you’re thinking what to say.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> It saves time</t>
+  </si>
+  <si>
+    <t>First we need to build a tool to do it.</t>
+  </si>
+  <si>
+    <t>This involves a lot of work.</t>
+  </si>
+  <si>
+    <t>electrons can move to higher energy states</t>
+  </si>
+  <si>
+    <t>by absorbing energy</t>
+  </si>
+  <si>
+    <t>There is nothing wrong with going back to your Year 11 information on bath houses,</t>
+  </si>
+  <si>
+    <t>because the activities that happened in one bath house generally happened in every other bath house.</t>
+  </si>
+  <si>
+    <t>Do, you know, are the themes of their artwork reflecting it?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> So it’s saying remember when we started, we said that Pompeii had originally been settled by Greeks? Okay?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> So it’s saying </t>
+  </si>
+  <si>
+    <t xml:space="preserve">remember </t>
+  </si>
+  <si>
+    <t>when we started</t>
+  </si>
+  <si>
+    <t>that Pompeii had originally been settled by Greeks? Okay?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">we said </t>
+  </si>
+  <si>
+    <t>Clause_4</t>
+  </si>
+  <si>
+    <t>Clause_5</t>
+  </si>
+  <si>
+    <t>Clause_6</t>
+  </si>
+  <si>
+    <t>High-Density lipoprotein (hdl) protects the artery wall by removing cholesterol from lipidladen macrophages.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> However, recent evidence suggests that hdl might also inhibit atherogenesis by combating inflammation.</t>
+  </si>
+  <si>
+    <t>High-Density lipoprotein (hdl) protects the artery wall</t>
+  </si>
+  <si>
+    <t>It doesn’t always have to be eight</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> by removing cholesterol from lipidladen macrophages.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> However, recent evidence suggests that hdl might also inhibit atherogenesis</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> by combating inflammation.</t>
+  </si>
+  <si>
+    <t>This column is going to be very small</t>
+  </si>
+  <si>
+    <t>if we look at where Italy is,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> it’s not that far from Egypt at this time</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> but atoms would like to have eight.</t>
+  </si>
+  <si>
+    <t>To identify potential anti-inflammatory mechanisms</t>
+  </si>
+  <si>
+    <t>we challenged macrophages with lipopolysaccharide, an inflammatory microbial ligand for Toll-like receptor 4.</t>
+  </si>
+  <si>
+    <t>because it’s just a number.</t>
+  </si>
+  <si>
+    <t>If you are disappointed with the number,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> then it means you probably could have tried a little bit harder, </t>
+  </si>
+  <si>
+    <t>You have to read it</t>
+  </si>
+  <si>
+    <t>and then you’re asked some questions</t>
+  </si>
+  <si>
+    <t>before sleeping in until lunchtime</t>
+  </si>
+  <si>
+    <t>The corn is fried</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> and then added to the mix.</t>
+  </si>
+  <si>
+    <t>Place the potatoes in the oven.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bake for thirty minutes.</t>
+  </si>
+  <si>
+    <t>he worked late at night</t>
+  </si>
+  <si>
+    <t>Egypt is part of the Roman Empire.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> So there would be massive amounts of trade going on,</t>
+  </si>
+  <si>
+    <t>You only have to do it one day,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> and then you’ve done your service.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> before sleeping in until lunchtime without attending lectures.</t>
+  </si>
+  <si>
+    <t>He took the mark</t>
+  </si>
+  <si>
+    <t>and kicked the goal</t>
+  </si>
+  <si>
+    <t>he liked rocking backwards and forwards in his chair,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">whilst thinking, </t>
+  </si>
+  <si>
+    <t>until the whole building shook.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> until the whole building shook.</t>
+  </si>
+  <si>
+    <t>he liked rocking backwards and forwards in his chair, whilst thinking,</t>
+  </si>
+  <si>
+    <t>you’ve got a written source</t>
+  </si>
+  <si>
+    <t>The scale is red, orange, yellow, green, blue, indigo, violet.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> David—where’s your gear?</t>
+  </si>
+  <si>
+    <t>you wouldn’t have heard this word before</t>
+  </si>
+  <si>
+    <t>When you get trade in ideas—</t>
+  </si>
+  <si>
+    <t>we call it aesthetic trade</t>
+  </si>
+  <si>
+    <t>It doesn’t look like this arrangement here.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> So we’ll just turn the lights on again</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> It doesn’t look like a full spectrum up here</t>
+  </si>
+  <si>
+    <t>you’ve got a picture source</t>
+  </si>
+  <si>
+    <t>We’re very pleased to open our season with a win.</t>
+  </si>
+  <si>
+    <t>We made sure they couldn’t run their attack and we managed to hold them down.</t>
+  </si>
+  <si>
+    <t>We made sure they couldn’t run their attack</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> we managed to hold them down.</t>
+  </si>
+  <si>
+    <t>They weren’t deflected at all.</t>
+  </si>
+  <si>
+    <t>Let us look at the example of element carbon in its ground (least energetic) state.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> It has 6 electrons.</t>
+  </si>
+  <si>
+    <t>hdl inhibits a subset of lipopolysaccharide-stimulated macrophage genes that regulate the type I interferon response,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> it's action is independent of sterol metabolism.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Most of them weren’t deflected at all? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I don’t think it’s a good idea for us. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> we shouldn’t go.</t>
+  </si>
+  <si>
+    <t>it doesn’t look like this arrangement here.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> It doesn’t look like a full spectrum up here. </t>
+  </si>
+  <si>
+    <t>Most of them weren’t deflected at all?</t>
+  </si>
+  <si>
+    <t>This is an example of an interrupting clause. There is a consequential link between 'When you get trade in ideas' and 'we call it aesthetic trade', but the clause 'you wouldn't have heard this word before' interrupts this link, in a way that we call incoherent sequencing.</t>
+  </si>
+  <si>
+    <t>It doesn’t look like this arrangement here.  So we’ll just turn the lights on again. It doesn’t look like a full spectrum up here</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -372,6 +681,12 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -441,6 +756,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Yaegan Doran" id="{BE9C5F95-BED8-4B57-BEB1-C7BE99648FE9}" userId="S::yadoran@acu.edu.au::f5e2410b-e174-4ac8-b7a7-e90ad6d33057" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -726,25 +1047,45 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="E10" dT="2023-10-11T03:53:13.03" personId="{BE9C5F95-BED8-4B57-BEB1-C7BE99648FE9}" id="{1470665B-3C43-41A1-9498-59EEAB91EE88}">
+    <text>In each of these chunks, there is in fact another consequential happening - the 'however' links the two chunks here in columns E and F, while the two 'by's link columns G&amp;H and I&amp;J.</text>
+  </threadedComment>
+  <threadedComment ref="E24" dT="2023-10-11T03:57:02.03" personId="{BE9C5F95-BED8-4B57-BEB1-C7BE99648FE9}" id="{7913A9A6-8C82-4B82-AC9C-24D09A33D601}">
+    <text>This example has two sets of links, linking three clauses - marked by 'whilst', linking column G&amp;H and 'until', linking columns G&amp;H with I.</text>
+  </threadedComment>
+  <threadedComment ref="E26" dT="2023-10-11T03:58:57.12" personId="{BE9C5F95-BED8-4B57-BEB1-C7BE99648FE9}" id="{EF522E50-4973-42D2-8A25-BF3CD1DC3959}">
+    <text>This is an example of an interrupting clause. There is a consequential link between 'When you get trade in ideas' and 'we call it aesthetic trade', but the clause 'you wouldn't have heard this word before' interrupts this link, in a way that we call incoherent sequencing.</text>
+  </threadedComment>
+  <threadedComment ref="D27" dT="2023-10-11T03:59:47.32" personId="{BE9C5F95-BED8-4B57-BEB1-C7BE99648FE9}" id="{5BD9D394-8FAF-477F-B0FD-7B00E365AEEC}">
+    <text>The  |INC… INC| is an annotation of the text, not part of the text itself. Should be removed from the transcript.</text>
+  </threadedComment>
+  <threadedComment ref="E27" dT="2023-10-11T04:01:22.34" personId="{BE9C5F95-BED8-4B57-BEB1-C7BE99648FE9}" id="{CA7BA8EC-4175-4884-91FD-DC948338054D}">
+    <text>As above, this involves an interrupting clause. The is a reiterative relation between 'It doesn't look like this arrangement here' and 'It doesn't look like a full spectrum here', but the clause 'So we'll just turn the lights on again' interrupts this, in a way we label incoherent sequencing.</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="22" customWidth="1"/>
     <col min="4" max="4" width="80" style="3" customWidth="1"/>
-    <col min="5" max="5" width="43.33203125" customWidth="1"/>
-    <col min="6" max="6" width="47.6640625" customWidth="1"/>
-    <col min="7" max="7" width="57.33203125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="20" customWidth="1"/>
+    <col min="5" max="5" width="43.33203125" style="3" customWidth="1"/>
+    <col min="6" max="12" width="47.6640625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="57.33203125" style="3" customWidth="1"/>
+    <col min="14" max="14" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -757,20 +1098,38 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>110</v>
+      <c r="E1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -783,14 +1142,29 @@
       <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="E2" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>108</v>
+      </c>
       <c r="G2" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H2" t="s">
+      <c r="N2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="192" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -803,15 +1177,26 @@
       <c r="D3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>112</v>
+      </c>
       <c r="G3" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="N3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -822,16 +1207,28 @@
         <v>12</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="M4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="N4" t="s">
         <v>17</v>
       </c>
-      <c r="H4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -844,14 +1241,26 @@
       <c r="D5" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="E5" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="G5" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="M5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H5" t="s">
+      <c r="N5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -864,619 +1273,947 @@
       <c r="D6" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="E6" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>118</v>
+      </c>
       <c r="G6" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="N6" t="s">
         <v>22</v>
       </c>
-      <c r="H6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:14" ht="96" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>120</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H8" t="s">
+        <v>121</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="M8" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+      <c r="N8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>124</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H9" t="s">
+        <v>123</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="M9" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="N9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="176" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>134</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H10" t="s">
+        <v>135</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="M10" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="N10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="160" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>142</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="H11" t="s">
+        <v>141</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="M11" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="176" x14ac:dyDescent="0.2">
+      <c r="N11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="128" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="E12" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="M12" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="H12" t="s">
+      <c r="N12" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="160" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" ht="144" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>43</v>
       </c>
+      <c r="E13" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>145</v>
+      </c>
       <c r="G13" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="M13" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="128" x14ac:dyDescent="0.2">
+      <c r="N13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="112" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>146</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H14" t="s">
+        <v>140</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="M14" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="144" x14ac:dyDescent="0.2">
+      <c r="N14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="112" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>48</v>
       </c>
+      <c r="E15" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>148</v>
+      </c>
       <c r="G15" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="M15" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="H15" t="s">
+      <c r="N15" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="112" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>150</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="112" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="N16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="N17" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H17" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:14" ht="96" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>57</v>
       </c>
+      <c r="E18" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>155</v>
+      </c>
       <c r="G18" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="M18" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="H18" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="N18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="96" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D19" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="M19" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="N19" t="s">
         <v>61</v>
       </c>
-      <c r="H19" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:14" ht="192" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>62</v>
       </c>
+      <c r="E20" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>158</v>
+      </c>
       <c r="G20" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="M20" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="H20" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+      <c r="N20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="80" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>64</v>
       </c>
+      <c r="E21" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>160</v>
+      </c>
       <c r="G21" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="M21" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="H21" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="192" x14ac:dyDescent="0.2">
+      <c r="N21" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="112" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C22" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D22" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="M22" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="G22" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H22" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+      <c r="N22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C23" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="M23" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="N23" t="s">
         <v>70</v>
       </c>
-      <c r="H23" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="112" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:14" ht="96" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>71</v>
       </c>
+      <c r="E24" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>167</v>
+      </c>
       <c r="G24" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="M24" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="H24" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="N24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>6</v>
+        <v>74</v>
       </c>
       <c r="B25" t="s">
-        <v>26</v>
+        <v>75</v>
       </c>
       <c r="C25" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="G25" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="M25" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="64" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>74</v>
       </c>
-      <c r="H25" t="s">
+      <c r="B26" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="96" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" t="s">
-        <v>26</v>
-      </c>
       <c r="C26" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="D26" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="M26" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="N26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="96" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" t="s">
         <v>76</v>
       </c>
-      <c r="G26" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H26" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="32" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>79</v>
-      </c>
-      <c r="B27" t="s">
-        <v>80</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="D27" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="M27" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="N27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="96" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28" t="s">
         <v>82</v>
       </c>
-      <c r="G27" s="3" t="s">
+      <c r="D28" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" ht="80" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>79</v>
-      </c>
-      <c r="B28" t="s">
-        <v>80</v>
-      </c>
-      <c r="C28" t="s">
-        <v>81</v>
-      </c>
-      <c r="D28" s="3" t="s">
+      <c r="E28" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="M28" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="G28" s="3" t="s">
+      <c r="N28" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" t="s">
+        <v>82</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="H28" t="s">
+      <c r="E29" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="M29" s="3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" ht="96" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>79</v>
-      </c>
-      <c r="B29" t="s">
-        <v>80</v>
-      </c>
-      <c r="C29" t="s">
-        <v>81</v>
-      </c>
-      <c r="D29" s="3" t="s">
+      <c r="N29" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="112" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" t="s">
+        <v>75</v>
+      </c>
+      <c r="C30" t="s">
+        <v>82</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="G29" s="3" t="s">
+      <c r="E30" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="M30" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="H29" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="96" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>79</v>
-      </c>
-      <c r="B30" t="s">
-        <v>80</v>
-      </c>
-      <c r="C30" t="s">
+    </row>
+    <row r="31" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>74</v>
+      </c>
+      <c r="B31" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" t="s">
+        <v>82</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="E31" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="M31" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="G30" s="3" t="s">
+      <c r="N31" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="80" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>74</v>
+      </c>
+      <c r="B32" t="s">
         <v>91</v>
       </c>
-      <c r="H30" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="48" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>79</v>
-      </c>
-      <c r="B31" t="s">
-        <v>80</v>
-      </c>
-      <c r="C31" t="s">
-        <v>89</v>
-      </c>
-      <c r="D31" s="3" t="s">
+      <c r="C32" t="s">
         <v>92</v>
       </c>
-      <c r="G31" s="3" t="s">
+      <c r="D32" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="H31" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="112" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>79</v>
-      </c>
-      <c r="B32" t="s">
-        <v>80</v>
-      </c>
-      <c r="C32" t="s">
-        <v>89</v>
-      </c>
-      <c r="D32" s="3" t="s">
+      <c r="E32" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="M32" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="G32" s="3" t="s">
+    </row>
+    <row r="33" spans="1:14" ht="96" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>74</v>
+      </c>
+      <c r="B33" t="s">
+        <v>91</v>
+      </c>
+      <c r="C33" t="s">
+        <v>92</v>
+      </c>
+      <c r="D33" s="3" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" ht="48" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>79</v>
-      </c>
-      <c r="B33" t="s">
-        <v>80</v>
-      </c>
-      <c r="C33" t="s">
-        <v>89</v>
-      </c>
-      <c r="D33" s="3" t="s">
+      <c r="E33" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="M33" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="G33" s="3" t="s">
+      <c r="N33" t="s">
         <v>97</v>
       </c>
-      <c r="H33" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B34" t="s">
+        <v>91</v>
+      </c>
+      <c r="C34" t="s">
+        <v>92</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C34" t="s">
+      <c r="E34" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="M34" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D34" s="3" t="s">
+    </row>
+    <row r="35" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>74</v>
+      </c>
+      <c r="B35" t="s">
+        <v>91</v>
+      </c>
+      <c r="C35" t="s">
         <v>100</v>
       </c>
-      <c r="G34" s="3" t="s">
+      <c r="D35" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="M35" s="3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="96" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>79</v>
-      </c>
-      <c r="B35" t="s">
-        <v>98</v>
-      </c>
-      <c r="C35" t="s">
-        <v>99</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="H35" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="48" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>79</v>
-      </c>
-      <c r="B36" t="s">
-        <v>98</v>
-      </c>
-      <c r="C36" t="s">
-        <v>99</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="48" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>79</v>
-      </c>
-      <c r="B37" t="s">
-        <v>98</v>
-      </c>
-      <c r="C37" t="s">
-        <v>107</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>